<commit_message>
Increased min. via size, sent back to fab
</commit_message>
<xml_diff>
--- a/circuits/Manufacturer/unselected parts.xlsx
+++ b/circuits/Manufacturer/unselected parts.xlsx
@@ -43,6 +43,15 @@
     <t xml:space="preserve">OPEN_AUTOMATION:QFN-20_5X5MM(SI3402-B-GM)</t>
   </si>
   <si>
+    <t xml:space="preserve">SJ1,SJ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN_AUTOMATION:SJUMP</t>
+  </si>
+  <si>
     <t xml:space="preserve">J5</t>
   </si>
   <si>
@@ -52,13 +61,52 @@
     <t xml:space="preserve">CONNECTOR_PINHEADER_2.54MM:PINHEADER_2X09_P2.54MM_VERTICAL_SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">SJ1,SJ2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEN_AUTOMATION:SJUMP</t>
+    <t xml:space="preserve">C11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_100NF_1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPACITOR_SMD:C_1206_3216METRIC_PAD1.33X1.80MM_HANDSOLDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAT54C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PACKAGE_TO_SOT_SMD:SOT-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_1UF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPACITOR_SMD:C_0603_1608METRIC_PAD1.08X0.95MM_HANDSOLDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D_ZENER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE_SMD:D_SMB_HANDSOLDERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_1NF_1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_LMUN2211LT1G</t>
   </si>
   <si>
     <t xml:space="preserve">C2,C6</t>
@@ -70,28 +118,13 @@
     <t xml:space="preserve">CAPACITOR_TANTALUM_SMD:CP_EIA-6032-15_KEMET-U_PAD2.25X2.35MM_HANDSOLDER</t>
   </si>
   <si>
-    <t xml:space="preserve">C11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C_100NF_1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPACITOR_SMD:C_1206_3216METRIC_PAD1.33X1.80MM_HANDSOLDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C_1NF_1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAT54C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACKAGE_TO_SOT_SMD:SOT-23</t>
+    <t xml:space="preserve">D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE_SMD:D_SMC_HANDSOLDERING</t>
   </si>
   <si>
     <t xml:space="preserve">R32</t>
@@ -103,115 +136,82 @@
     <t xml:space="preserve">RESISTOR_SMD:R_0603_1608METRIC_PAD0.98X0.95MM_HANDSOLDER</t>
   </si>
   <si>
-    <t xml:space="preserve">D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D_ZENER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE_SMD:D_SMB_HANDSOLDERING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C_1UF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPACITOR_SMD:C_0603_1608METRIC_PAD1.08X0.95MM_HANDSOLDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1,Q3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q_MBT3904</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PACKAGE_TO_SOT_SMD:SOT-363_SC-70-6_HANDSOLDERING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q_LMUN2211LT1G</t>
+    <t xml:space="preserve">C16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_15UF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPACITOR_THT:CP_RADIAL_D6.3MM_P2.50MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARREL_JACK_OD5.5_ID2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN_AUTOMATION:BARRELJACK_OD5.5_ID2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB_MINI_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN_AUTOMATION:USB-MINI-B-0548190519</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1,J6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN_01X12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONNECTOR_PHOENIX_MC_HIGHVOLTAGE:PHOENIXCONTACT_MC_1,5_12-G-5.08_1X12_P5.08MM_HORIZONTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESIGNATOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOOTPRINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-3035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN_AUTOMATION:AI-3035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOUSING-MOUNTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN_AUTOMATION:HOUSING-MOUNTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RJ45_LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONNECTOR_RJ:RJ45_ABRACON_ARJP11A-MA_HORIZONTAL</t>
   </si>
   <si>
     <t xml:space="preserve">C17</t>
   </si>
   <si>
     <t xml:space="preserve">C_680UF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPACITOR_THT:CP_RADIAL_D6.3MM_P2.50MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C_15UF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOUSING-MOUNTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEN_AUTOMATION:HOUSING-MOUNTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BARREL_JACK_OD5.5_ID2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEN_AUTOMATION:BARRELJACK_OD5.5_ID2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB_MINI_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEN_AUTOMATION:USB-MINI-B-0548190519</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESIGNATOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOOTPRINT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1,J6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONN_01X12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONNECTOR_PHOENIX_MC_HIGHVOLTAGE:PHOENIXCONTACT_MC_1,5_12-G-5.08_1X12_P5.08MM_HORIZONTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RJ45_LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONNECTOR_RJ:RJ45_ABRACON_ARJP11A-MA_HORIZONTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AI-3035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEN_AUTOMATION:AI-3035</t>
   </si>
   <si>
     <t xml:space="preserve">J2,J3,J4,J7,J8,J9</t>
@@ -348,10 +348,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="99.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="18.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,7 +390,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,7 +404,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,7 +418,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,7 +443,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -454,13 +451,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -468,13 +465,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -488,7 +485,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -496,41 +493,41 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D12" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -558,7 +555,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
@@ -566,13 +563,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
@@ -580,13 +577,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
@@ -594,13 +591,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0</v>
@@ -608,13 +605,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0</v>
@@ -622,13 +619,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
@@ -636,13 +633,13 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -650,13 +647,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>

</xml_diff>